<commit_message>
filter short data update
</commit_message>
<xml_diff>
--- a/Print.xlsx
+++ b/Print.xlsx
@@ -586,7 +586,7 @@
       </c>
       <c r="E2" s="17" t="inlineStr">
         <is>
-          <t>LAVANYA</t>
+          <t>KAMLESH</t>
         </is>
       </c>
       <c r="F2" s="18" t="n"/>
@@ -613,7 +613,7 @@
       </c>
       <c r="B4" s="10" t="inlineStr">
         <is>
-          <t>6(6*4)</t>
+          <t>1078(3/2)</t>
         </is>
       </c>
       <c r="C4" s="1" t="n"/>
@@ -652,7 +652,7 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>28/01/2022</t>
+          <t>0000-00-00</t>
         </is>
       </c>
       <c r="C5" s="1" t="n"/>
@@ -662,17 +662,17 @@
       </c>
       <c r="F5" s="9" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>245</t>
         </is>
       </c>
       <c r="G5" s="9" t="inlineStr">
         <is>
-          <t>LICHI</t>
+          <t>CREKAL</t>
         </is>
       </c>
       <c r="H5" s="9" t="inlineStr">
         <is>
-          <t>CREAM</t>
+          <t>CHIKU</t>
         </is>
       </c>
       <c r="I5" s="1" t="n"/>
@@ -685,7 +685,7 @@
       </c>
       <c r="B6" s="10" t="inlineStr">
         <is>
-          <t>M100</t>
+          <t>M45</t>
         </is>
       </c>
       <c r="C6" s="1" t="n"/>
@@ -695,17 +695,17 @@
       </c>
       <c r="F6" s="9" t="inlineStr">
         <is>
-          <t>210</t>
+          <t>245</t>
         </is>
       </c>
       <c r="G6" s="9" t="inlineStr">
         <is>
-          <t>COLOR-JUTH</t>
+          <t>CREKAL</t>
         </is>
       </c>
       <c r="H6" s="9" t="inlineStr">
         <is>
-          <t>GREY</t>
+          <t>CHIKU</t>
         </is>
       </c>
       <c r="I6" s="1" t="n"/>
@@ -718,7 +718,7 @@
       </c>
       <c r="B7" s="10" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>56</t>
         </is>
       </c>
       <c r="C7" s="1" t="n"/>
@@ -728,17 +728,17 @@
       </c>
       <c r="F7" s="8" t="inlineStr">
         <is>
-          <t>210</t>
+          <t>330</t>
         </is>
       </c>
       <c r="G7" s="9" t="inlineStr">
         <is>
-          <t>EGAL</t>
+          <t>JUTH</t>
         </is>
       </c>
       <c r="H7" s="9" t="inlineStr">
         <is>
-          <t>CHAMPION</t>
+          <t>VFD9723</t>
         </is>
       </c>
       <c r="I7" s="1" t="n"/>
@@ -759,9 +759,21 @@
       <c r="E8" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F8" s="8" t="inlineStr"/>
-      <c r="G8" s="9" t="inlineStr"/>
-      <c r="H8" s="9" t="inlineStr"/>
+      <c r="F8" s="8" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="G8" s="9" t="inlineStr">
+        <is>
+          <t>MX</t>
+        </is>
+      </c>
+      <c r="H8" s="9" t="inlineStr">
+        <is>
+          <t>PAL MAT</t>
+        </is>
+      </c>
       <c r="I8" s="1" t="n"/>
     </row>
     <row r="9" ht="15.6" customHeight="1" s="16">
@@ -771,7 +783,7 @@
         </is>
       </c>
       <c r="B9" s="10" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1" t="n"/>
       <c r="D9" s="1" t="n"/>
@@ -791,7 +803,7 @@
       </c>
       <c r="B10" s="10" t="inlineStr">
         <is>
-          <t>66</t>
+          <t>60</t>
         </is>
       </c>
       <c r="C10" s="1" t="n"/>

</xml_diff>